<commit_message>
Updated testcases for failing results and all URL
</commit_message>
<xml_diff>
--- a/Excel/Test_Data.xlsx
+++ b/Excel/Test_Data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Praful_Personal\GitProject\AMPS_Automation\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nayan.thakor\Documents\PersonalWorkspace\AMPS_Automation\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C61EF8E-0A15-42B9-80E7-63EBE8307272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="847"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="847" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="7" r:id="rId1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="134">
   <si>
     <t>Project Name</t>
   </si>
@@ -421,13 +422,28 @@
     <t>Contact Log</t>
   </si>
   <si>
-    <t>environment1</t>
+    <t>environmentALT</t>
+  </si>
+  <si>
+    <t>environmentDOT</t>
+  </si>
+  <si>
+    <t>environmentROW</t>
+  </si>
+  <si>
+    <t>environmentALTROW</t>
+  </si>
+  <si>
+    <t>geoamps sample project</t>
+  </si>
+  <si>
+    <t>geoamps sample project-00005</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -501,7 +517,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -533,35 +549,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -842,11 +844,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -879,7 +881,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>128</v>
+        <v>56</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>55</v>
@@ -890,7 +892,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>128</v>
+        <v>56</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>46</v>
@@ -899,18 +901,78 @@
         <v>60</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{1B0503A3-F233-4A45-99A9-9CC5C5B78FC1}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{70143AFD-395A-47A0-B51A-BB46AC62809F}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{E68587A7-37AC-4E23-95F2-DF6369CAE736}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{9A539BE9-E873-415A-B532-B7098F76EAA8}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{62845B04-6973-427A-B724-C686F51BCE0E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -919,128 +981,127 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" style="17" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="17" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" style="17" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" style="17" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="17" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="17"/>
+    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="16" t="s">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="3" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" t="s">
         <v>84</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" t="s">
         <v>88</v>
       </c>
-      <c r="D3" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="17" t="s">
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" t="s">
         <v>83</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" t="s">
         <v>87</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="17" t="s">
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" t="s">
         <v>83</v>
       </c>
-      <c r="F4" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" s="17" t="s">
+      <c r="F4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+      <c r="A5" t="s">
         <v>86</v>
       </c>
-      <c r="B5" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="17" t="s">
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
         <v>88</v>
       </c>
-      <c r="E5" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="17" t="s">
+      <c r="E5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1050,7 +1111,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1060,110 +1121,110 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="22" customWidth="1"/>
-    <col min="4" max="4" width="19" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="17" customWidth="1"/>
+    <col min="4" max="4" width="19" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="19" t="s">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="15" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="16" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="17">
         <v>12345</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="17" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" t="s">
         <v>94</v>
       </c>
-      <c r="B4" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="21" t="s">
+      <c r="B4" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="17" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+      <c r="A5" t="s">
         <v>95</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="17">
         <v>45678</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="F5" s="21" t="s">
+      <c r="F5" s="17" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1173,7 +1234,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1215,7 +1276,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1291,7 +1352,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1366,7 +1427,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1556,11 +1617,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1673,10 +1734,10 @@
         <v>74</v>
       </c>
       <c r="G4" t="s">
-        <v>75</v>
+        <v>132</v>
       </c>
       <c r="H4" t="s">
-        <v>76</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1711,7 +1772,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1759,7 +1820,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1867,7 +1928,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2006,7 +2067,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2023,41 +2084,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="18" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" t="s">
         <v>108</v>
       </c>
       <c r="B3" s="12">
@@ -2074,7 +2135,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" t="s">
         <v>109</v>
       </c>
       <c r="B4" s="12">

</xml_diff>

<commit_message>
Updated environment details and single browser execution for each env
</commit_message>
<xml_diff>
--- a/Excel/Test_Data.xlsx
+++ b/Excel/Test_Data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Praful_Personal\GitProject\AMPS_Automation\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nayan.thakor\Documents\PersonalWorkspace\AMPS_Automation\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C3DE546-BD57-4C6F-999C-765E6DCEFAD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="847" firstSheet="4" activeTab="9"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="847" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="7" r:id="rId1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="138">
   <si>
     <t>Project Name</t>
   </si>
@@ -205,9 +206,6 @@
     <t>https://uat.geoamps.com/dotAMPS/Login/Login.aspx</t>
   </si>
   <si>
-    <t>environment</t>
-  </si>
-  <si>
     <t>ENV</t>
   </si>
   <si>
@@ -427,12 +425,6 @@
     <t>environmentALTROW</t>
   </si>
   <si>
-    <t>geoamps sample project</t>
-  </si>
-  <si>
-    <t>geoamps sample project-00005</t>
-  </si>
-  <si>
     <t>environmentALTDOT</t>
   </si>
   <si>
@@ -443,12 +435,27 @@
   </si>
   <si>
     <t>Engineer</t>
+  </si>
+  <si>
+    <t>Document Generation</t>
+  </si>
+  <si>
+    <t>Testing 1</t>
+  </si>
+  <si>
+    <t>Testing 1-123</t>
+  </si>
+  <si>
+    <t>Test project 1</t>
+  </si>
+  <si>
+    <t>Test project 1-00001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -849,186 +856,283 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
     <col min="2" max="2" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B2" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C2" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="11" t="s">
+      <c r="B3" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C3" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" s="11" t="s">
+      <c r="B4" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C4" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" s="11" t="s">
+      <c r="B5" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="C5" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B7" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" s="10" t="s">
+      <c r="C9" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="D10" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B11" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="C11" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
         <v>129</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>133</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>55</v>
       </c>
       <c r="C12" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>60</v>
+      <c r="D14" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B7" r:id="rId6"/>
-    <hyperlink ref="B8" r:id="rId7"/>
-    <hyperlink ref="B9" r:id="rId8"/>
-    <hyperlink ref="B10" r:id="rId9"/>
-    <hyperlink ref="B11" r:id="rId10"/>
-    <hyperlink ref="B12" r:id="rId11"/>
-    <hyperlink ref="B13" r:id="rId12"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B12" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B14" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -1063,47 +1167,47 @@
         <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>81</v>
-      </c>
       <c r="D2" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" t="s">
         <v>82</v>
       </c>
-      <c r="C3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D3" t="s">
-        <v>83</v>
-      </c>
       <c r="E3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C4" t="s">
         <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E4" t="s">
         <v>35</v>
@@ -1111,19 +1215,19 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E5" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1132,7 +1236,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1174,44 +1278,44 @@
         <v>12</v>
       </c>
       <c r="B2" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>104</v>
-      </c>
       <c r="D2" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E2" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="F2" s="16" t="s">
         <v>99</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C3" s="17">
         <v>12345</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>35</v>
@@ -1231,22 +1335,22 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C5" s="17">
         <v>45678</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1255,7 +1359,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1280,15 +1384,15 @@
         <v>12</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1297,11 +1401,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="B1" sqref="B1:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1373,7 +1477,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1448,7 +1552,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1618,7 +1722,7 @@
         <v>35</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>36</v>
@@ -1638,18 +1742,18 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.28515625" customWidth="1"/>
     <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
@@ -1688,103 +1792,103 @@
         <v>12</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>66</v>
-      </c>
       <c r="E2" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>70</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>71</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" t="s">
         <v>67</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>68</v>
       </c>
-      <c r="D3" t="s">
-        <v>69</v>
-      </c>
       <c r="E3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" t="s">
         <v>73</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>74</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>75</v>
-      </c>
-      <c r="H3" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E4" t="s">
+        <v>133</v>
+      </c>
+      <c r="F4" t="s">
         <v>73</v>
       </c>
-      <c r="F4" t="s">
-        <v>74</v>
-      </c>
       <c r="G4" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="H4" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" t="s">
         <v>73</v>
       </c>
-      <c r="F5" t="s">
-        <v>74</v>
-      </c>
       <c r="G5" t="s">
-        <v>75</v>
+        <v>136</v>
       </c>
       <c r="H5" t="s">
-        <v>76</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -1793,7 +1897,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1823,7 +1927,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
@@ -1841,7 +1945,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1886,15 +1990,15 @@
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>14</v>
@@ -1911,7 +2015,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>14</v>
@@ -1928,7 +2032,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>14</v>
@@ -1949,7 +2053,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2003,18 +2107,18 @@
         <v>19</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>113</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>17</v>
@@ -2037,7 +2141,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>17</v>
@@ -2060,7 +2164,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>17</v>
@@ -2088,7 +2192,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2126,21 +2230,21 @@
         <v>12</v>
       </c>
       <c r="B2" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="D2" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="E2" s="18" t="s">
         <v>110</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B3" s="12">
         <v>44805</v>
@@ -2157,7 +2261,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B4" s="12">
         <v>44805</v>

</xml_diff>